<commit_message>
Restart spreadsheets as new
Had issue with different column names
</commit_message>
<xml_diff>
--- a/Output - Vyne Spreadsheets/Vyne S3A.xlsx
+++ b/Output - Vyne Spreadsheets/Vyne S3A.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,15 +446,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Price</t>
+          <t>Price Current</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Price Previous</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Price Change</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Change Status</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Date Available</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Scrape Datetime</t>
         </is>

</xml_diff>